<commit_message>
base para a comunicação do banco de dados com a interface
</commit_message>
<xml_diff>
--- a/automacoes.xlsx
+++ b/automacoes.xlsx
@@ -1,41 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>bom dia</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -53,25 +45,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -359,22 +416,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>boa tarde</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ar da sala</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>boa tarde</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ar da sala</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>boa tarde</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ar da sala</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando parametrização p/ planilhas e correções gerais
</commit_message>
<xml_diff>
--- a/automacoes.xlsx
+++ b/automacoes.xlsx
@@ -1,39 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+  <si>
+    <t>boa tarde</t>
+  </si>
+  <si>
+    <t>ar da sala</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -45,90 +72,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,87 +390,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>boa tarde</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
         <v>5</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ar da sala</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
         <v>23</v>
       </c>
-      <c r="E1" t="b">
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>boa tarde</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ar da sala</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2">
         <v>23</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>boa tarde</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ar da sala</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>23</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correções de bugs na comunicação com o banco de dados das automações
</commit_message>
<xml_diff>
--- a/automacoes.xlsx
+++ b/automacoes.xlsx
@@ -1,66 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
-  <si>
-    <t>boa tarde</t>
-  </si>
-  <si>
-    <t>ar da sala</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -72,37 +45,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -390,55 +416,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ar da sala</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Boa tarde</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Tv da sala</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>52</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Hora de estudar</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ar da cozinha</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hora do almoço</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ar do quarto</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>19</v>
+      </c>
+      <c r="E4" t="b">
         <v>0</v>
-      </c>
-      <c r="B1" s="2">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2">
-        <v>23</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>